<commit_message>
add Aaron's devliery date
</commit_message>
<xml_diff>
--- a/01_doc/wpr_log/refine_checklist.xlsx
+++ b/01_doc/wpr_log/refine_checklist.xlsx
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -247,6 +247,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,11 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -587,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -602,7 +604,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -617,7 +619,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -632,7 +634,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -647,7 +649,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -660,9 +662,11 @@
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -675,9 +679,11 @@
       <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -690,9 +696,11 @@
       <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E8" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -703,9 +711,11 @@
       <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -718,9 +728,11 @@
       <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E10" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -733,9 +745,11 @@
       <c r="D11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="42.75" hidden="1" x14ac:dyDescent="0.15">
+      <c r="E11" s="13">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -750,7 +764,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="28.5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -765,7 +779,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -778,7 +792,9 @@
       <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="13">
+        <v>42004</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
@@ -795,7 +811,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -855,7 +871,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -885,7 +901,7 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -898,7 +914,9 @@
       <c r="D22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="13">
+        <v>42009</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
@@ -915,7 +933,7 @@
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -930,7 +948,7 @@
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -945,7 +963,7 @@
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -990,7 +1008,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1006,13 +1024,7 @@
       <c r="E29" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="许林"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
add new doc structure
</commit_message>
<xml_diff>
--- a/01_doc/wpr_log/refine_checklist.xlsx
+++ b/01_doc/wpr_log/refine_checklist.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="check_list" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="52">
   <si>
     <t>ITEM NO#</t>
   </si>
@@ -135,17 +135,57 @@
   </si>
   <si>
     <t>JavaScript使用Jquery风格</t>
+  </si>
+  <si>
+    <t>需求跟踪矩阵</t>
+  </si>
+  <si>
+    <t>模块-&gt;功能-&gt;需求规格说明书-&gt;概要设计说明书-&gt;详细设计说明书-&gt;测试用例</t>
+  </si>
+  <si>
+    <t>需求规格说明书</t>
+  </si>
+  <si>
+    <t>保持现有需求文档
+增加补充部分需求</t>
+  </si>
+  <si>
+    <t>从原有架构文档中拆出4个视图，逻辑视图（系统架构图），物理视图（网络拓扑图），开发视图（描述系统分层模型，WEB前端技术，数据库选型，应用服务器选型，项目管理工具，测试方法论），数据视图（ER图）</t>
+  </si>
+  <si>
+    <t>概要设计说明书</t>
+  </si>
+  <si>
+    <t>由系统功能模块图出发，对每个模块的功能定义进行说明，对实现这个功能的技术进行描述；模块之间的数据流；系统接口定义；数据库设计（数据字典）</t>
+  </si>
+  <si>
+    <t>开发设计规范</t>
+  </si>
+  <si>
+    <t>见编码规则，改名即可</t>
+  </si>
+  <si>
+    <t>详细设计说明书</t>
+  </si>
+  <si>
+    <t>开发环境配置，项目目录结构，模块详细开发说明</t>
+  </si>
+  <si>
+    <t>TBH</t>
+  </si>
+  <si>
+    <t>架构设计说明书</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -172,7 +212,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -231,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -280,9 +320,18 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -298,7 +347,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -340,7 +389,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +424,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,23 +633,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -617,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -634,7 +683,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -651,7 +700,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -668,7 +717,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -685,7 +734,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -702,7 +751,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -719,7 +768,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -736,22 +785,22 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:5" ht="14.25">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="13">
-        <v>42004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="E9" s="15">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -768,7 +817,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -785,7 +834,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -802,7 +851,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="14.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -819,7 +868,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -836,7 +885,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -851,7 +900,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -868,7 +917,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -885,7 +934,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="14.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -902,7 +951,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -919,7 +968,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -936,7 +985,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -953,7 +1002,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -970,7 +1019,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="14.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -987,7 +1036,7 @@
         <v>42016</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1004,7 +1053,7 @@
         <v>42019</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1021,7 +1070,7 @@
         <v>42019</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1038,7 +1087,7 @@
         <v>42019</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="14.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1053,7 +1102,7 @@
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="14.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1068,7 +1117,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="14.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1085,7 +1134,7 @@
         <v>42009</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="14.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1100,6 +1149,90 @@
       </c>
       <c r="E30" s="13">
         <v>42004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27">
+      <c r="B32" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="27">
+      <c r="B33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="54">
+      <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="40.5">
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="14.25">
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="14.25">
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1247,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D30</xm:sqref>
+          <xm:sqref>D2:D30 D32:D37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1138,16 +1271,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1163,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1171,7 +1304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1187,22 +1320,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="C8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="C9" t="s">
         <v>24</v>
       </c>

</xml_diff>